<commit_message>
feat: Slug por cliente + Onboarding + Manual
</commit_message>
<xml_diff>
--- a/Planilha de vendas - Teste 2.xlsx
+++ b/Planilha de vendas - Teste 2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automatizar input vendas - CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06B5BE5-1B03-4D08-87EC-E69E0E7ADCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56792DA-E2C5-4FC5-8A41-A1AECAB71639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25500" yWindow="465" windowWidth="21630" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$A$1:$K$993</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$A$1:$K$992</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>DATA ATENDIMENTO</t>
   </si>
@@ -66,18 +66,6 @@
   </si>
   <si>
     <t>VENCIMENTO</t>
-  </si>
-  <si>
-    <t>TESTE 1</t>
-  </si>
-  <si>
-    <t>TESTE 2</t>
-  </si>
-  <si>
-    <t>TESTE 3</t>
-  </si>
-  <si>
-    <t>TESTE 4</t>
   </si>
   <si>
     <t>Receita de Consulta</t>
@@ -119,9 +107,6 @@
     <t>1x</t>
   </si>
   <si>
-    <t>5x</t>
-  </si>
-  <si>
     <t>10x</t>
   </si>
   <si>
@@ -132,6 +117,18 @@
   </si>
   <si>
     <t>Prestação de serviços estéticos</t>
+  </si>
+  <si>
+    <t>TESTE 5</t>
+  </si>
+  <si>
+    <t>TESTE 6</t>
+  </si>
+  <si>
+    <t>TESTE 7</t>
+  </si>
+  <si>
+    <t>TESTE 8</t>
   </si>
 </sst>
 </file>
@@ -611,21 +608,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y993"/>
+  <dimension ref="A1:Y992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
@@ -633,12 +630,12 @@
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -684,19 +681,19 @@
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>46041</v>
+        <v>46042</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2" s="10">
         <v>1</v>
@@ -705,16 +702,16 @@
         <v>200</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K2" s="6">
-        <v>46041</v>
+        <v>46042</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
@@ -733,19 +730,19 @@
     </row>
     <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>46041</v>
+        <v>46042</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -754,16 +751,16 @@
         <v>200</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K3" s="6">
-        <v>46041</v>
+        <v>46042</v>
       </c>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
@@ -782,37 +779,37 @@
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>46041</v>
+        <v>46043</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="11">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K4" s="6">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -831,37 +828,37 @@
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>46041</v>
+        <v>46043</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="11">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>27</v>
-      </c>
       <c r="K5" s="6">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -880,37 +877,37 @@
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>46040</v>
+        <v>46044</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="11">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K6" s="6">
-        <v>46071</v>
+        <v>46075</v>
       </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -929,37 +926,37 @@
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>46040</v>
+        <v>46045</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="11">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K7" s="6">
-        <v>46071</v>
+        <v>46045</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -977,39 +974,17 @@
       <c r="Y7" s="15"/>
     </row>
     <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>46039</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="10">
-        <v>1</v>
-      </c>
-      <c r="G8" s="11">
-        <v>250</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="6">
-        <v>46039</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
@@ -1133,12 +1108,12 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="10"/>
       <c r="G13" s="11"/>
       <c r="H13" s="12"/>
@@ -1165,7 +1140,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="10"/>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
@@ -1415,20 +1390,20 @@
       <c r="I23" s="13"/>
       <c r="J23" s="14"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
@@ -1570,7 +1545,7 @@
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="12"/>
@@ -1597,7 +1572,7 @@
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
       <c r="H30" s="12"/>
@@ -1975,7 +1950,7 @@
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="9"/>
+      <c r="E44" s="8"/>
       <c r="F44" s="10"/>
       <c r="G44" s="11"/>
       <c r="H44" s="12"/>
@@ -2002,7 +1977,7 @@
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="12"/>
@@ -2407,7 +2382,7 @@
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
-      <c r="E60" s="9"/>
+      <c r="E60" s="8"/>
       <c r="F60" s="10"/>
       <c r="G60" s="11"/>
       <c r="H60" s="12"/>
@@ -2434,7 +2409,7 @@
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="E61" s="9"/>
       <c r="F61" s="10"/>
       <c r="G61" s="11"/>
       <c r="H61" s="12"/>
@@ -2515,11 +2490,11 @@
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="10"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="12"/>
       <c r="G64" s="11"/>
       <c r="H64" s="12"/>
-      <c r="I64" s="13"/>
+      <c r="I64" s="8"/>
       <c r="J64" s="14"/>
       <c r="K64" s="6"/>
       <c r="L64" s="5"/>
@@ -2569,7 +2544,7 @@
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="E66" s="9"/>
       <c r="F66" s="12"/>
       <c r="G66" s="11"/>
       <c r="H66" s="12"/>
@@ -2704,7 +2679,7 @@
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
-      <c r="E71" s="9"/>
+      <c r="E71" s="8"/>
       <c r="F71" s="12"/>
       <c r="G71" s="11"/>
       <c r="H71" s="12"/>
@@ -2762,7 +2737,7 @@
       <c r="F73" s="12"/>
       <c r="G73" s="11"/>
       <c r="H73" s="12"/>
-      <c r="I73" s="8"/>
+      <c r="I73" s="13"/>
       <c r="J73" s="14"/>
       <c r="K73" s="6"/>
       <c r="L73" s="5"/>
@@ -2790,7 +2765,7 @@
       <c r="G74" s="11"/>
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
-      <c r="J74" s="14"/>
+      <c r="J74" s="11"/>
       <c r="K74" s="6"/>
       <c r="L74" s="5"/>
       <c r="M74" s="5"/>
@@ -2817,7 +2792,7 @@
       <c r="G75" s="11"/>
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
-      <c r="J75" s="11"/>
+      <c r="J75" s="14"/>
       <c r="K75" s="6"/>
       <c r="L75" s="5"/>
       <c r="M75" s="5"/>
@@ -2839,7 +2814,7 @@
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+      <c r="E76" s="9"/>
       <c r="F76" s="12"/>
       <c r="G76" s="11"/>
       <c r="H76" s="12"/>
@@ -2893,7 +2868,7 @@
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
-      <c r="E78" s="9"/>
+      <c r="E78" s="8"/>
       <c r="F78" s="12"/>
       <c r="G78" s="11"/>
       <c r="H78" s="12"/>
@@ -2951,7 +2926,7 @@
       <c r="F80" s="12"/>
       <c r="G80" s="11"/>
       <c r="H80" s="12"/>
-      <c r="I80" s="13"/>
+      <c r="I80" s="8"/>
       <c r="J80" s="14"/>
       <c r="K80" s="6"/>
       <c r="L80" s="5"/>
@@ -2978,7 +2953,7 @@
       <c r="F81" s="12"/>
       <c r="G81" s="11"/>
       <c r="H81" s="12"/>
-      <c r="I81" s="8"/>
+      <c r="I81" s="13"/>
       <c r="J81" s="14"/>
       <c r="K81" s="6"/>
       <c r="L81" s="5"/>
@@ -3001,7 +2976,7 @@
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
+      <c r="E82" s="9"/>
       <c r="F82" s="12"/>
       <c r="G82" s="11"/>
       <c r="H82" s="12"/>
@@ -3028,11 +3003,11 @@
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
-      <c r="E83" s="9"/>
+      <c r="E83" s="8"/>
       <c r="F83" s="12"/>
       <c r="G83" s="11"/>
       <c r="H83" s="12"/>
-      <c r="I83" s="13"/>
+      <c r="I83" s="8"/>
       <c r="J83" s="14"/>
       <c r="K83" s="6"/>
       <c r="L83" s="5"/>
@@ -3194,7 +3169,7 @@
       <c r="F89" s="12"/>
       <c r="G89" s="11"/>
       <c r="H89" s="12"/>
-      <c r="I89" s="8"/>
+      <c r="I89" s="13"/>
       <c r="J89" s="14"/>
       <c r="K89" s="6"/>
       <c r="L89" s="5"/>
@@ -3240,15 +3215,15 @@
       <c r="Y90" s="5"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="17"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
       <c r="F91" s="12"/>
-      <c r="G91" s="11"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="12"/>
-      <c r="I91" s="13"/>
+      <c r="I91" s="8"/>
       <c r="J91" s="14"/>
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
@@ -3267,16 +3242,16 @@
       <c r="Y91" s="5"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="18"/>
+      <c r="A92" s="6"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="20"/>
       <c r="H92" s="12"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="14"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
       <c r="M92" s="5"/>
@@ -3294,13 +3269,13 @@
       <c r="Y92" s="5"/>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="19"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="20"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="23"/>
       <c r="H93" s="12"/>
       <c r="I93" s="11"/>
       <c r="J93" s="11"/>
@@ -3321,13 +3296,13 @@
       <c r="Y93" s="5"/>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A94" s="16"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="23"/>
+      <c r="A94" s="6"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="20"/>
       <c r="H94" s="12"/>
       <c r="I94" s="11"/>
       <c r="J94" s="11"/>
@@ -3620,8 +3595,8 @@
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="19"/>
-      <c r="C105" s="12"/>
-      <c r="D105" s="12"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
       <c r="E105" s="12"/>
       <c r="F105" s="19"/>
       <c r="G105" s="20"/>
@@ -3672,13 +3647,13 @@
       <c r="Y106" s="5"/>
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="20"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="24"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="23"/>
       <c r="H107" s="12"/>
       <c r="I107" s="11"/>
       <c r="J107" s="11"/>
@@ -3699,13 +3674,13 @@
       <c r="Y107" s="5"/>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="21"/>
-      <c r="C108" s="24"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="23"/>
+      <c r="A108" s="6"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="20"/>
       <c r="H108" s="12"/>
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
@@ -3755,8 +3730,8 @@
     <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="19"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
       <c r="E110" s="12"/>
       <c r="F110" s="19"/>
       <c r="G110" s="20"/>
@@ -3836,7 +3811,7 @@
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="19"/>
-      <c r="C113" s="12"/>
+      <c r="C113" s="8"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
       <c r="F113" s="19"/>
@@ -3863,9 +3838,9 @@
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="B114" s="19"/>
-      <c r="C114" s="8"/>
+      <c r="C114" s="12"/>
       <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
+      <c r="E114" s="8"/>
       <c r="F114" s="19"/>
       <c r="G114" s="20"/>
       <c r="H114" s="12"/>
@@ -3890,9 +3865,9 @@
     <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
       <c r="B115" s="19"/>
-      <c r="C115" s="12"/>
+      <c r="C115" s="8"/>
       <c r="D115" s="12"/>
-      <c r="E115" s="8"/>
+      <c r="E115" s="12"/>
       <c r="F115" s="19"/>
       <c r="G115" s="20"/>
       <c r="H115" s="12"/>
@@ -3917,9 +3892,9 @@
     <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
       <c r="B116" s="19"/>
-      <c r="C116" s="8"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
+      <c r="E116" s="8"/>
       <c r="F116" s="19"/>
       <c r="G116" s="20"/>
       <c r="H116" s="12"/>
@@ -3944,9 +3919,9 @@
     <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="B117" s="19"/>
-      <c r="C117" s="12"/>
+      <c r="C117" s="8"/>
       <c r="D117" s="12"/>
-      <c r="E117" s="8"/>
+      <c r="E117" s="12"/>
       <c r="F117" s="19"/>
       <c r="G117" s="20"/>
       <c r="H117" s="12"/>
@@ -3971,9 +3946,9 @@
     <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
       <c r="B118" s="19"/>
-      <c r="C118" s="8"/>
+      <c r="C118" s="12"/>
       <c r="D118" s="12"/>
-      <c r="E118" s="12"/>
+      <c r="E118" s="8"/>
       <c r="F118" s="19"/>
       <c r="G118" s="20"/>
       <c r="H118" s="12"/>
@@ -3998,9 +3973,9 @@
     <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="B119" s="19"/>
-      <c r="C119" s="12"/>
+      <c r="C119" s="8"/>
       <c r="D119" s="12"/>
-      <c r="E119" s="8"/>
+      <c r="E119" s="12"/>
       <c r="F119" s="19"/>
       <c r="G119" s="20"/>
       <c r="H119" s="12"/>
@@ -4025,7 +4000,7 @@
     <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
       <c r="B120" s="19"/>
-      <c r="C120" s="8"/>
+      <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
       <c r="F120" s="19"/>
@@ -4160,7 +4135,7 @@
     <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="19"/>
-      <c r="C125" s="12"/>
+      <c r="C125" s="8"/>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
       <c r="F125" s="19"/>
@@ -4293,17 +4268,17 @@
       <c r="Y129" s="5"/>
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
-      <c r="B130" s="19"/>
-      <c r="C130" s="8"/>
-      <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="20"/>
-      <c r="H130" s="12"/>
-      <c r="I130" s="11"/>
-      <c r="J130" s="11"/>
-      <c r="K130" s="6"/>
+      <c r="A130" s="25"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="26"/>
+      <c r="E130" s="26"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="27"/>
+      <c r="H130" s="26"/>
+      <c r="I130" s="27"/>
+      <c r="J130" s="27"/>
+      <c r="K130" s="25"/>
       <c r="L130" s="5"/>
       <c r="M130" s="5"/>
       <c r="N130" s="5"/>
@@ -7641,31 +7616,17 @@
       <c r="Y253" s="5"/>
     </row>
     <row r="254" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A254" s="25"/>
-      <c r="B254" s="15"/>
-      <c r="C254" s="26"/>
-      <c r="D254" s="26"/>
-      <c r="E254" s="26"/>
-      <c r="F254" s="15"/>
-      <c r="G254" s="27"/>
-      <c r="H254" s="26"/>
-      <c r="I254" s="27"/>
-      <c r="J254" s="27"/>
-      <c r="K254" s="25"/>
-      <c r="L254" s="5"/>
-      <c r="M254" s="5"/>
-      <c r="N254" s="5"/>
-      <c r="O254" s="5"/>
-      <c r="P254" s="5"/>
-      <c r="Q254" s="5"/>
-      <c r="R254" s="5"/>
-      <c r="S254" s="5"/>
-      <c r="T254" s="5"/>
-      <c r="U254" s="5"/>
-      <c r="V254" s="5"/>
-      <c r="W254" s="5"/>
-      <c r="X254" s="5"/>
-      <c r="Y254" s="5"/>
+      <c r="A254" s="28"/>
+      <c r="B254" s="29"/>
+      <c r="C254" s="30"/>
+      <c r="D254" s="30"/>
+      <c r="E254" s="30"/>
+      <c r="F254" s="29"/>
+      <c r="G254" s="31"/>
+      <c r="H254" s="30"/>
+      <c r="I254" s="29"/>
+      <c r="J254" s="29"/>
+      <c r="K254" s="32"/>
     </row>
     <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A255" s="28"/>
@@ -7694,17 +7655,17 @@
       <c r="K256" s="32"/>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A257" s="28"/>
-      <c r="B257" s="29"/>
-      <c r="C257" s="30"/>
-      <c r="D257" s="30"/>
-      <c r="E257" s="30"/>
-      <c r="F257" s="29"/>
-      <c r="G257" s="31"/>
-      <c r="H257" s="30"/>
-      <c r="I257" s="29"/>
-      <c r="J257" s="29"/>
-      <c r="K257" s="32"/>
+      <c r="A257" s="33"/>
+      <c r="B257" s="34"/>
+      <c r="C257" s="35"/>
+      <c r="D257" s="35"/>
+      <c r="E257" s="35"/>
+      <c r="F257" s="36"/>
+      <c r="G257" s="37"/>
+      <c r="H257" s="35"/>
+      <c r="I257" s="34"/>
+      <c r="J257" s="34"/>
+      <c r="K257" s="38"/>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="33"/>
@@ -8643,17 +8604,17 @@
       <c r="K329" s="38"/>
     </row>
     <row r="330" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A330" s="33"/>
+      <c r="A330" s="39"/>
       <c r="B330" s="34"/>
-      <c r="C330" s="35"/>
-      <c r="D330" s="35"/>
-      <c r="E330" s="35"/>
+      <c r="C330" s="34"/>
+      <c r="D330" s="34"/>
+      <c r="E330" s="34"/>
       <c r="F330" s="36"/>
       <c r="G330" s="37"/>
-      <c r="H330" s="35"/>
+      <c r="H330" s="34"/>
       <c r="I330" s="34"/>
       <c r="J330" s="34"/>
-      <c r="K330" s="38"/>
+      <c r="K330" s="40"/>
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="39"/>
@@ -17261,21 +17222,11 @@
       <c r="J992" s="34"/>
       <c r="K992" s="40"/>
     </row>
-    <row r="993" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A993" s="39"/>
-      <c r="B993" s="34"/>
-      <c r="C993" s="34"/>
-      <c r="D993" s="34"/>
-      <c r="E993" s="34"/>
-      <c r="F993" s="36"/>
-      <c r="G993" s="37"/>
-      <c r="H993" s="34"/>
-      <c r="I993" s="34"/>
-      <c r="J993" s="34"/>
-      <c r="K993" s="40"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K993" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K992" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y994">
+    <sortCondition ref="B2:B994"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>